<commit_message>
test cases are added for -ve fields validation, beforeeach test in the sheet
</commit_message>
<xml_diff>
--- a/Postman API automation/Contact Us and API Automation Test Cases.xlsx
+++ b/Postman API automation/Contact Us and API Automation Test Cases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Postman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Postman\Assignments\Postman API automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="UI Automation" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
   <si>
     <t>TC no</t>
   </si>
@@ -439,6 +439,55 @@
   <si>
     <t>1. validate assertion status code 200 returned on response
 2. run the test through as collection and select .csv file and verify that defined by_id and by+type data response is geneatd</t>
+  </si>
+  <si>
+    <t>Locator Management</t>
+  </si>
+  <si>
+    <t>Before and Aftereach to load URL</t>
+  </si>
+  <si>
+    <t>Contact Us -&gt; Field validation</t>
+  </si>
+  <si>
+    <t>Add locator for each field on contact us page</t>
+  </si>
+  <si>
+    <t>Add locator for each field on contact us page - all contact us fields
+1. first name, last name, phone number, email id, message etc</t>
+  </si>
+  <si>
+    <t>all locators are added to the fields and data is getting added on the all fields</t>
+  </si>
+  <si>
+    <t>Write a BeforeEach annotation for URL</t>
+  </si>
+  <si>
+    <t>1. Add beforeEach Annotation for URL 
+2. verify ULR will get launch for each test cases</t>
+  </si>
+  <si>
+    <t>contact us URL is getting launch successfully for each URL</t>
+  </si>
+  <si>
+    <t>Add assertion for all fields when there is no data entered on the fields</t>
+  </si>
+  <si>
+    <t>1. Enter text into the phone number or enter phone number less than 10 digits, and validate assertion
+2. Enter text instead email address validate assertion
+3. enter blank data into firstname, lastname, message field and validate assertion text</t>
+  </si>
+  <si>
+    <t>All fields has been asserted successfully on not entering the data</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>TC9</t>
   </si>
 </sst>
 </file>
@@ -497,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -521,6 +570,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,15 +857,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.88671875" customWidth="1"/>
     <col min="4" max="4" width="54.88671875" customWidth="1"/>
     <col min="5" max="5" width="49.77734375" customWidth="1"/>
@@ -944,7 +999,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -960,6 +1015,66 @@
         <v>70</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -972,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,7 +1176,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="288" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
@@ -1181,7 +1296,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>93</v>
       </c>

</xml_diff>